<commit_message>
fixed bugs in excel tables
</commit_message>
<xml_diff>
--- a/Excel/Grade.xlsx
+++ b/Excel/Grade.xlsx
@@ -984,13 +984,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1311,20 +1311,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9" style="16"/>
     <col min="2" max="2" width="19.125" style="16" customWidth="1"/>
     <col min="3" max="3" width="32.125" style="16" customWidth="1"/>
-    <col min="4" max="9" width="18.625" style="16" customWidth="1"/>
-    <col min="10" max="16380" width="9" style="16"/>
-    <col min="16383" max="16384" width="9" style="16"/>
+    <col min="4" max="4" width="18.625" style="16" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="16"/>
   </cols>
   <sheetData>
     <row r="1" ht="26" customHeight="1" spans="1:4">
@@ -1341,7 +1340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:4">
       <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
@@ -1354,16 +1353,15 @@
       <c r="D2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="17"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="16" t="s">
@@ -1374,10 +1372,10 @@
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="16" t="s">
@@ -1388,10 +1386,10 @@
       <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="16" t="s">
@@ -1402,10 +1400,10 @@
       <c r="A6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="16" t="s">
@@ -1416,10 +1414,10 @@
       <c r="A7" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="19" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="16" t="s">
@@ -1430,10 +1428,10 @@
       <c r="A8" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="19" t="s">
         <v>28</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -1444,10 +1442,10 @@
       <c r="A9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="19" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -1458,10 +1456,10 @@
       <c r="A10" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="19" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -1472,10 +1470,10 @@
       <c r="A11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="C11" s="19" t="s">
         <v>40</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -1486,10 +1484,10 @@
       <c r="A12" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C12" s="19" t="s">
         <v>44</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -1500,262 +1498,12 @@
       <c r="A13" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="14" spans="2:3">
-      <c r="B14" s="19"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="2:3">
-      <c r="B15" s="19"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="19"/>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="19"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="19"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="19"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="19"/>
-      <c r="C22" s="17"/>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="19"/>
-      <c r="C23" s="17"/>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="19"/>
-      <c r="C24" s="17"/>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="19"/>
-      <c r="C25" s="17"/>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="19"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="19"/>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="19"/>
-      <c r="C28" s="17"/>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="19"/>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="19"/>
-      <c r="C30" s="17"/>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="19"/>
-      <c r="C31" s="17"/>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="19"/>
-      <c r="C32" s="17"/>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="19"/>
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="19"/>
-      <c r="C34" s="17"/>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="19"/>
-      <c r="C35" s="17"/>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="19"/>
-      <c r="C36" s="17"/>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="19"/>
-      <c r="C37" s="17"/>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="19"/>
-      <c r="C38" s="17"/>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="19"/>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="19"/>
-      <c r="C40" s="17"/>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="19"/>
-      <c r="C41" s="17"/>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="19"/>
-      <c r="C42" s="17"/>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="19"/>
-      <c r="C43" s="17"/>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="19"/>
-      <c r="C44" s="17"/>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="19"/>
-      <c r="C45" s="17"/>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="19"/>
-      <c r="C46" s="17"/>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="19"/>
-      <c r="C47" s="17"/>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" s="19"/>
-      <c r="C48" s="17"/>
-    </row>
-    <row r="49" spans="2:3">
-      <c r="B49" s="19"/>
-      <c r="C49" s="17"/>
-    </row>
-    <row r="50" spans="3:3">
-      <c r="C50" s="17"/>
-    </row>
-    <row r="51" spans="3:3">
-      <c r="C51" s="17"/>
-    </row>
-    <row r="52" spans="3:3">
-      <c r="C52" s="17"/>
-    </row>
-    <row r="53" spans="3:3">
-      <c r="C53" s="17"/>
-    </row>
-    <row r="54" spans="3:3">
-      <c r="C54" s="17"/>
-    </row>
-    <row r="55" spans="3:3">
-      <c r="C55" s="17"/>
-    </row>
-    <row r="56" spans="3:3">
-      <c r="C56" s="17"/>
-    </row>
-    <row r="57" spans="3:3">
-      <c r="C57" s="17"/>
-    </row>
-    <row r="58" spans="3:3">
-      <c r="C58" s="17"/>
-    </row>
-    <row r="59" spans="3:3">
-      <c r="C59" s="17"/>
-    </row>
-    <row r="60" spans="3:3">
-      <c r="C60" s="17"/>
-    </row>
-    <row r="61" spans="3:3">
-      <c r="C61" s="17"/>
-    </row>
-    <row r="62" spans="3:3">
-      <c r="C62" s="17"/>
-    </row>
-    <row r="63" spans="3:3">
-      <c r="C63" s="17"/>
-    </row>
-    <row r="64" spans="3:3">
-      <c r="C64" s="17"/>
-    </row>
-    <row r="65" spans="3:3">
-      <c r="C65" s="17"/>
-    </row>
-    <row r="66" spans="3:3">
-      <c r="C66" s="17"/>
-    </row>
-    <row r="67" spans="3:3">
-      <c r="C67" s="17"/>
-    </row>
-    <row r="68" spans="3:3">
-      <c r="C68" s="17"/>
-    </row>
-    <row r="69" spans="3:3">
-      <c r="C69" s="17"/>
-    </row>
-    <row r="70" spans="3:3">
-      <c r="C70" s="17"/>
-    </row>
-    <row r="71" spans="3:3">
-      <c r="C71" s="17"/>
-    </row>
-    <row r="72" spans="2:3">
-      <c r="B72" s="17"/>
-      <c r="C72" s="17"/>
-    </row>
-    <row r="73" spans="3:3">
-      <c r="C73" s="17"/>
-    </row>
-    <row r="74" spans="3:3">
-      <c r="C74" s="17"/>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75" s="19"/>
-      <c r="C75" s="17"/>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76" s="19"/>
-      <c r="C76" s="17"/>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77" s="19"/>
-      <c r="C77" s="17"/>
-    </row>
-    <row r="78" spans="2:3">
-      <c r="B78" s="19"/>
-      <c r="C78" s="17"/>
-    </row>
-    <row r="79" spans="2:3">
-      <c r="B79" s="19"/>
-      <c r="C79" s="17"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="18"/>
-      <c r="B80" s="19"/>
-      <c r="C80" s="17"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="18"/>
-      <c r="B81" s="19"/>
-      <c r="C81" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>